<commit_message>
addded curavture info for incourse
</commit_message>
<xml_diff>
--- a/区間情報/区間情報インコースまとめ.xlsx
+++ b/区間情報/区間情報インコースまとめ.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="20130" windowHeight="8610" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="20130" windowHeight="8595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="数値データ" sheetId="1" r:id="rId1"/>
     <sheet name="コース図" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>ベーシック</t>
     <phoneticPr fontId="1"/>
@@ -206,10 +206,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>null</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>InFifthStraight</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -228,6 +224,18 @@
   </si>
   <si>
     <t>InSixthCurve_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>638?</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -852,15 +860,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:colOff>102291</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:rowOff>119684</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>226116</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>60049</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -869,8 +877,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1457325" y="3286126"/>
-          <a:ext cx="809625" cy="285749"/>
+          <a:off x="1477204" y="3424445"/>
+          <a:ext cx="811282" cy="288234"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3432,7 +3440,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3499,7 +3507,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F4" s="4">
         <v>1800</v>
@@ -3575,19 +3583,20 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
-        <v>32</v>
+      <c r="D9">
+        <f>I9*(PI()/180)*G9</f>
+        <v>1193.8052083641214</v>
       </c>
       <c r="G9">
         <v>90</v>
       </c>
       <c r="H9">
-        <f>1/1050.17</f>
-        <v>9.5222678233047972E-4</v>
+        <f>1/760</f>
+        <v>1.3157894736842105E-3</v>
       </c>
       <c r="I9">
         <f>1/H9</f>
-        <v>1050.17</v>
+        <v>760</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -3610,19 +3619,20 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
-        <v>32</v>
+      <c r="D11">
+        <f>I11*(PI()/180)*G11</f>
+        <v>761.8362184955248</v>
       </c>
       <c r="G11">
         <v>90</v>
       </c>
       <c r="H11">
-        <f>1/726.76</f>
-        <v>1.3759700588915186E-3</v>
+        <f>1/485</f>
+        <v>2.0618556701030928E-3</v>
       </c>
       <c r="I11">
         <f>1/H11</f>
-        <v>726.76</v>
+        <v>485</v>
       </c>
       <c r="K11" s="4"/>
     </row>
@@ -3631,20 +3641,21 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
-        <v>32</v>
+      <c r="D12">
+        <f>I12*PI()/180*G12</f>
+        <v>447.97191378013258</v>
       </c>
       <c r="G12">
-        <f>90-9.34</f>
-        <v>80.66</v>
+        <f>90-20.63</f>
+        <v>69.37</v>
       </c>
       <c r="H12">
-        <f>1/(12.91*51.912)</f>
-        <v>1.49212771324027E-3</v>
+        <f>1/(370)</f>
+        <v>2.7027027027027029E-3</v>
       </c>
       <c r="I12">
         <f>1/H12</f>
-        <v>670.18391999999994</v>
+        <v>370</v>
       </c>
       <c r="J12">
         <v>570</v>
@@ -3656,22 +3667,21 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
+      <c r="D13">
+        <f>I13*PI()/180*G13</f>
+        <v>299.32571204627948</v>
       </c>
       <c r="G13">
-        <v>40.869999999999997</v>
+        <f>27.34+24.63</f>
+        <v>51.97</v>
       </c>
       <c r="H13">
-        <f>1/(17.86*51.912)</f>
-        <v>1.0785760793914831E-3</v>
+        <f>1/330</f>
+        <v>3.0303030303030303E-3</v>
       </c>
       <c r="I13">
         <f>1/H13</f>
-        <v>927.14831999999979</v>
+        <v>330</v>
       </c>
       <c r="J13">
         <v>527</v>
@@ -3686,6 +3696,9 @@
       <c r="D14">
         <v>575</v>
       </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
       <c r="H14">
         <v>0</v>
       </c>
@@ -3777,7 +3790,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G19">
         <f>2.67+28.57</f>
@@ -3846,7 +3859,7 @@
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23">
         <v>140</v>
@@ -3869,7 +3882,7 @@
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -3888,7 +3901,7 @@
     <row r="25" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25">
         <v>50</v>
@@ -3900,7 +3913,7 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
         <v>32</v>
@@ -3922,7 +3935,7 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
@@ -3959,7 +3972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
No merge In and Out
</commit_message>
<xml_diff>
--- a/区間情報/区間情報インコースまとめ.xlsx
+++ b/区間情報/区間情報インコースまとめ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="20130" windowHeight="8610" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="20130" windowHeight="8595"/>
   </bookViews>
   <sheets>
     <sheet name="数値データ" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>ベーシック</t>
     <phoneticPr fontId="1"/>
@@ -214,20 +214,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>inFifthCurve</t>
+    <t>InSixthCurve</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">AfterinFiftCurveStraight
-</t>
+    <t>AfterFifthCureveStraight</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>InSixthCurve_1</t>
+    <t>InFifthCurve_2</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>InSixthCurve_2</t>
+    <t>InFifthCurve_1</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1341,16 +1340,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>588644</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>160002</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>626744</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>17127</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1359,7 +1358,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4886325" y="3238500"/>
+          <a:off x="5610225" y="4981575"/>
           <a:ext cx="502919" cy="7602"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2340,16 +2339,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>18318</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>65943</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>134815</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>242523</xdr:colOff>
+      <xdr:rowOff>106240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>290148</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>86458</xdr:rowOff>
+      <xdr:rowOff>57883</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2358,7 +2357,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5504718" y="4592515"/>
+          <a:off x="6238143" y="4563940"/>
           <a:ext cx="910005" cy="465993"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2389,7 +2388,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
-            <a:t>OutFifth</a:t>
+            <a:t>InFifth</a:t>
           </a:r>
           <a:br>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
@@ -2455,7 +2454,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
-            <a:t>OutSixth</a:t>
+            <a:t>InSixth</a:t>
           </a:r>
           <a:br>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0"/>
@@ -2472,16 +2471,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>92320</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>103309</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>618393</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>24179</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>82795</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>122359</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>608868</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>43229</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2490,7 +2489,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4892920" y="3532309"/>
+          <a:off x="5569195" y="5094409"/>
           <a:ext cx="526073" cy="263770"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2530,16 +2529,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>164124</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>41763</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>4397</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>134083</xdr:rowOff>
+      <xdr:colOff>116499</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>60813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>642572</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>153133</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2548,7 +2547,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4964724" y="2613513"/>
+          <a:off x="5602899" y="4347063"/>
           <a:ext cx="526073" cy="263770"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3431,8 +3430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K13"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3561,7 +3560,7 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>390</v>
+        <v>345</v>
       </c>
       <c r="F8">
         <v>378.6</v>
@@ -3849,11 +3848,10 @@
         <v>34</v>
       </c>
       <c r="D23">
-        <v>140</v>
+        <v>320</v>
       </c>
       <c r="F23">
-        <f>SUM(D23)</f>
-        <v>140</v>
+        <v>320</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -3869,17 +3867,16 @@
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="D24">
+        <v>413</v>
       </c>
       <c r="G24">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H24">
-        <f>1/I23</f>
-        <v>2.136752136752137E-3</v>
+        <v>-3.8025799999999998E-3</v>
       </c>
       <c r="I24">
         <v>650</v>
@@ -3888,10 +3885,16 @@
     <row r="25" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D25">
-        <v>50</v>
+        <v>592</v>
+      </c>
+      <c r="G25">
+        <v>48</v>
+      </c>
+      <c r="H25">
+        <v>-1.1633100000000001E-3</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -3900,17 +3903,10 @@
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26">
-        <v>90</v>
-      </c>
-      <c r="H26">
-        <f>1/I26</f>
-        <v>2.2727272727272726E-3</v>
+        <v>36</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
       </c>
       <c r="I26">
         <v>440</v>
@@ -3922,17 +3918,16 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="D27">
+        <v>2231</v>
       </c>
       <c r="G27">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="H27">
-        <f>1/I27</f>
-        <v>1.7241379310344827E-3</v>
+        <v>8.5315499999999997E-4</v>
       </c>
       <c r="I27">
         <v>580</v>
@@ -3959,7 +3954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>

</xml_diff>